<commit_message>
Excel dynamic panel can render column or row numbers
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataReaderRenderTest/TestRenderDataReader.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataReaderRenderTest/TestRenderDataReader.xlsx
@@ -172,13 +172,17 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="6">
+  <x:cellXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -492,13 +496,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:Q6"/>
+  <x:dimension ref="A1:V7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:17">
+    <x:row r="2" spans="1:22">
       <x:c r="B2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -518,63 +522,83 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:17">
+    <x:row r="3" spans="1:22">
       <x:c r="B3" s="2" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="s">
+      <x:c r="C3" s="2" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="n">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D3" s="2" t="b">
+    </x:row>
+    <x:row r="4" spans="1:22">
+      <x:c r="B4" s="3" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C4" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D4" s="3" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="E3" s="2" t="s"/>
-      <x:c r="F3" s="2" t="s"/>
-      <x:c r="G3" s="3" t="n">
+      <x:c r="E4" s="3" t="s"/>
+      <x:c r="F4" s="3" t="s"/>
+      <x:c r="G4" s="4" t="n">
         <x:v>523635.93</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:17">
-      <x:c r="B4" s="2" t="n">
+    <x:row r="5" spans="1:22">
+      <x:c r="B5" s="3" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C4" s="2" t="s">
+      <x:c r="C5" s="3" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D4" s="2" t="b">
+      <x:c r="D5" s="3" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E4" s="2" t="n">
+      <x:c r="E5" s="3" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="F4" s="2" t="s">
+      <x:c r="F5" s="3" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="G4" s="3" t="s"/>
+      <x:c r="G5" s="4" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:17">
-      <x:c r="B5" s="2" t="n">
+    <x:row r="6" spans="1:22">
+      <x:c r="B6" s="3" t="n">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C5" s="2" t="s">
+      <x:c r="C6" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D5" s="2" t="s"/>
-      <x:c r="E5" s="2" t="s"/>
-      <x:c r="F5" s="2" t="s">
+      <x:c r="D6" s="3" t="s"/>
+      <x:c r="E6" s="3" t="s"/>
+      <x:c r="F6" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G5" s="3" t="n">
+      <x:c r="G6" s="4" t="n">
         <x:v>100000.5532</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:17">
-      <x:c r="B6" s="5" t="s"/>
-      <x:c r="C6" s="5" t="s"/>
-      <x:c r="D6" s="5" t="s"/>
-      <x:c r="E6" s="5" t="s"/>
-      <x:c r="F6" s="5" t="s"/>
-      <x:c r="G6" s="4" t="n">
+    <x:row r="7" spans="1:22">
+      <x:c r="B7" s="6" t="s"/>
+      <x:c r="C7" s="6" t="s"/>
+      <x:c r="D7" s="6" t="s"/>
+      <x:c r="E7" s="6" t="s"/>
+      <x:c r="F7" s="6" t="s"/>
+      <x:c r="G7" s="5" t="n">
         <x:v>623636.4832</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Fix error while rendering when a cell contains unknown formula
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataReaderRenderTest/TestRenderDataReader.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataReaderRenderTest/TestRenderDataReader.xlsx
@@ -82,7 +82,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="4">
+  <x:borders count="5">
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
@@ -151,8 +151,25 @@
         <x:color rgb="FF000000"/>
       </x:diagonal>
     </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="dashed">
+        <x:color rgb="FF0000FF"/>
+      </x:left>
+      <x:right style="dashed">
+        <x:color rgb="FF0000FF"/>
+      </x:right>
+      <x:top style="dashed">
+        <x:color rgb="FF0000FF"/>
+      </x:top>
+      <x:bottom style="dashed">
+        <x:color rgb="FF0000FF"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="6">
+  <x:cellStyleXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -171,8 +188,11 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="7">
+  <x:cellXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -198,6 +218,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -496,7 +520,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:V7"/>
+  <x:dimension ref="A1:V9"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -602,6 +626,11 @@
         <x:v>623636.4832</x:v>
       </x:c>
     </x:row>
+    <x:row r="9" spans="1:22">
+      <x:c r="B9" s="7">
+        <x:f>COLUMN()</x:f>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Migrate to the newest version of Closed.XML
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataReaderRenderTest/TestRenderDataReader.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DataSourceDynamicPanelDataReaderRenderTest/TestRenderDataReader.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -55,7 +55,7 @@
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="165" formatCode="#,0.00"/>
+    <x:numFmt numFmtId="164" formatCode="#,0.00"/>
   </x:numFmts>
   <x:fonts count="2">
     <x:font>
@@ -179,13 +179,13 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -209,15 +209,15 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -520,13 +520,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:V9"/>
+  <x:dimension ref="A1:G9"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:22">
+    <x:row r="2" spans="1:7">
       <x:c r="B2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -546,28 +546,28 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:22">
-      <x:c r="B3" s="2" t="n">
+    <x:row r="3" spans="1:7">
+      <x:c r="B3" s="2">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="n">
+      <x:c r="C3" s="2">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D3" s="2" t="n">
+      <x:c r="D3" s="2">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E3" s="2" t="n">
+      <x:c r="E3" s="2">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F3" s="2" t="n">
+      <x:c r="F3" s="2">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G3" s="2" t="n">
+      <x:c r="G3" s="2">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:22">
-      <x:c r="B4" s="3" t="n">
+    <x:row r="4" spans="1:7">
+      <x:c r="B4" s="3">
         <x:v>1</x:v>
       </x:c>
       <x:c r="C4" s="3" t="s">
@@ -576,14 +576,14 @@
       <x:c r="D4" s="3" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="E4" s="3" t="s"/>
-      <x:c r="F4" s="3" t="s"/>
-      <x:c r="G4" s="4" t="n">
+      <x:c r="E4" s="3"/>
+      <x:c r="F4" s="3"/>
+      <x:c r="G4" s="4">
         <x:v>523635.93</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:22">
-      <x:c r="B5" s="3" t="n">
+    <x:row r="5" spans="1:7">
+      <x:c r="B5" s="3">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C5" s="3" t="s">
@@ -592,41 +592,41 @@
       <x:c r="D5" s="3" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="E5" s="3" t="n">
+      <x:c r="E5" s="3">
         <x:v>1</x:v>
       </x:c>
       <x:c r="F5" s="3" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="G5" s="4" t="s"/>
+      <x:c r="G5" s="4"/>
     </x:row>
-    <x:row r="6" spans="1:22">
-      <x:c r="B6" s="3" t="n">
+    <x:row r="6" spans="1:7">
+      <x:c r="B6" s="3">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D6" s="3" t="s"/>
-      <x:c r="E6" s="3" t="s"/>
+      <x:c r="D6" s="3"/>
+      <x:c r="E6" s="3"/>
       <x:c r="F6" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="G6" s="4" t="n">
+      <x:c r="G6" s="4">
         <x:v>100000.5532</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:22">
-      <x:c r="B7" s="6" t="s"/>
-      <x:c r="C7" s="6" t="s"/>
-      <x:c r="D7" s="6" t="s"/>
-      <x:c r="E7" s="6" t="s"/>
-      <x:c r="F7" s="6" t="s"/>
-      <x:c r="G7" s="5" t="n">
+    <x:row r="7" spans="1:7">
+      <x:c r="B7" s="5"/>
+      <x:c r="C7" s="5"/>
+      <x:c r="D7" s="5"/>
+      <x:c r="E7" s="5"/>
+      <x:c r="F7" s="5"/>
+      <x:c r="G7" s="6">
         <x:v>623636.4832</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:22">
+    <x:row r="9" spans="1:7">
       <x:c r="B9" s="7">
         <x:f>COLUMN()</x:f>
       </x:c>

</xml_diff>